<commit_message>
Baselines regression and BruteForce Classification
</commit_message>
<xml_diff>
--- a/results/Baselines.xlsx
+++ b/results/Baselines.xlsx
@@ -5,86 +5,120 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classification" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Regression" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
-  <si>
-    <t>AUROC</t>
-  </si>
-  <si>
-    <t>AUCPR</t>
-  </si>
-  <si>
-    <t>GLOBAL</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>TRA</t>
-  </si>
-  <si>
-    <t>VAL</t>
-  </si>
-  <si>
-    <t>TRAIN_VAL</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>birds</t>
-  </si>
-  <si>
-    <t>corel5k</t>
-  </si>
-  <si>
-    <t>emotions</t>
-  </si>
-  <si>
-    <t>yeast</t>
-  </si>
-  <si>
-    <t>flags</t>
-  </si>
-  <si>
-    <t>genbase</t>
-  </si>
-  <si>
-    <t>mediamill</t>
-  </si>
-  <si>
-    <t>LOCAL</t>
-  </si>
-  <si>
-    <t>Runtime LOCAL</t>
-  </si>
-  <si>
-    <t>Runtime GLOBAL</t>
-  </si>
-  <si>
-    <t>TRA-VAL</t>
-  </si>
-  <si>
-    <t>TRAVAL-TST</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">AUROC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUCPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLOBAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAIN_VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corel5k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emotions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yeast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediamill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime LOCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime GLOBAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRA-VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAVAL-TST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water-quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oes10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oes97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scm1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scm20d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rf1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rf2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -113,13 +147,40 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Abyssinica SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Abyssinica SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,6 +227,38 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,13 +281,13 @@
   </sheetPr>
   <dimension ref="B4:N46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,4 +979,999 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B4:M46"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5"/>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.892402857142857</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.902662857142857</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.892269285714285</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.901333571428571</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>1.51114142857143</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>1.55266214285714</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>1.51204571428571</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <v>1.54834428571429</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>255.93082125</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>306.15322625</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>253.61631875</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>335.522344375</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>437773.1889125</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>1017199.04916062</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>434855.2196625</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <v>1449696.48115875</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>421.09486125</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>553.82128125</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>406.55563625</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>507.864773125</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>964548.681049375</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>2585320.383625</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>776085.04768875</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <v>2114498.78511125</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>69.536618125</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>85.260905</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>67.875554375</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>79.86608875</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>10589.663829375</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>17471.2205975</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>10247.408909375</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>15357.2590825</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>78.458145</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>99.173618125</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>76.184513125</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>93.221359375</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>13895.73134625</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>23127.82743875</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>13299.18539875</v>
+      </c>
+      <c r="M14" s="5" t="n">
+        <v>20866.32091625</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>6.47229</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>6.68499625</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>5.27375375</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>5.4100575</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>303.02792125</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <v>307.068745</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>224.3894425</v>
+      </c>
+      <c r="M15" s="5" t="n">
+        <v>226.7312425</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>6.4946775</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>6.706185</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>5.290625</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>5.42545125</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>303.12952125</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>307.18629</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>224.46528</v>
+      </c>
+      <c r="M16" s="5" t="n">
+        <v>226.7945825</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="5"/>
+      <c r="C21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="5"/>
+      <c r="C24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="5"/>
+      <c r="C25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>1.01041</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>1.13053928571429</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0.9934</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>1.13028571428571</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="5" t="n">
+        <v>1.73263</v>
+      </c>
+      <c r="K25" s="5" t="n">
+        <v>2.15774857142857</v>
+      </c>
+      <c r="L25" s="5" t="n">
+        <v>1.69303</v>
+      </c>
+      <c r="M25" s="5" t="n">
+        <v>2.19085928571429</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="5"/>
+      <c r="C26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>57.80229</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>499.45816875</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>50.84133</v>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>491.31227625</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="5" t="n">
+        <v>24971.18424</v>
+      </c>
+      <c r="K26" s="5" t="n">
+        <v>3176851.47097187</v>
+      </c>
+      <c r="L26" s="5" t="n">
+        <v>16353.57148</v>
+      </c>
+      <c r="M26" s="5" t="n">
+        <v>3101817.93497875</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="5"/>
+      <c r="C27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>337.11928</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>1851.46832625</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>334.497</v>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>1753.382644375</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="5" t="n">
+        <v>1302586.73765</v>
+      </c>
+      <c r="K27" s="5" t="n">
+        <v>2040821.76565046</v>
+      </c>
+      <c r="L27" s="5" t="n">
+        <v>1245277.99081</v>
+      </c>
+      <c r="M27" s="5" t="n">
+        <v>2881910.1245609</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="5"/>
+      <c r="C28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>26.22968</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>300.634660625</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>25.93467</v>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>300.225634375</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="5" t="n">
+        <v>1948.76242</v>
+      </c>
+      <c r="K28" s="5" t="n">
+        <v>158327.485320625</v>
+      </c>
+      <c r="L28" s="5" t="n">
+        <v>1961.36357</v>
+      </c>
+      <c r="M28" s="5" t="n">
+        <v>157614.5850775</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="5"/>
+      <c r="C29" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>32.77307</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>301.95774125</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>30.29945</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>299.311493125</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="5" t="n">
+        <v>3029.01857</v>
+      </c>
+      <c r="K29" s="5" t="n">
+        <v>159389.516884375</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <v>2426.20854</v>
+      </c>
+      <c r="M29" s="5" t="n">
+        <v>157497.783911875</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="5"/>
+      <c r="C30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>0.63385</v>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>90.16980375</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>0.54231</v>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>90.07159</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="5" t="n">
+        <v>3.02781</v>
+      </c>
+      <c r="K30" s="5" t="n">
+        <v>13174.9925125</v>
+      </c>
+      <c r="L30" s="5" t="n">
+        <v>1.39634</v>
+      </c>
+      <c r="M30" s="5" t="n">
+        <v>13163.4386275</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5"/>
+      <c r="C31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>0.64947</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>90.1649525</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>0.58182</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>90.0847275</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <v>2.18155</v>
+      </c>
+      <c r="K31" s="5" t="n">
+        <v>13178.11955375</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <v>1.52552</v>
+      </c>
+      <c r="M31" s="5" t="n">
+        <v>13168.41406125</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="5"/>
+      <c r="C38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="5"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="5" t="n">
+        <v>0.9057863016</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <v>0.9462262891</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>0.7821255686</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>0.8245773513</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="5" t="n">
+        <v>4.2329055846</v>
+      </c>
+      <c r="D41" s="5" t="n">
+        <v>4.6374111585</v>
+      </c>
+      <c r="E41" s="5" t="n">
+        <v>1.3783522521</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>1.3186180735</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="5" t="n">
+        <v>2.9060312532</v>
+      </c>
+      <c r="D42" s="5" t="n">
+        <v>3.1518642212</v>
+      </c>
+      <c r="E42" s="5" t="n">
+        <v>1.181958891</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>1.2048076641</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="5" t="n">
+        <v>188.5734724373</v>
+      </c>
+      <c r="D43" s="5" t="n">
+        <v>212.9870482358</v>
+      </c>
+      <c r="E43" s="5" t="n">
+        <v>25.2891484259</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>27.8128212876</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="5" t="n">
+        <v>30.8752096612</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <v>34.080220889</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <v>5.8162083637</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>6.187034559</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="5" t="n">
+        <v>13.0235509585</v>
+      </c>
+      <c r="D45" s="5" t="n">
+        <v>14.238620308</v>
+      </c>
+      <c r="E45" s="5" t="n">
+        <v>3.7833076547</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>4.2317243036</v>
+      </c>
+      <c r="G45" s="5"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="5" t="n">
+        <v>127.589514254</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <v>137.4138773598</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>22.1240375491</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <v>25.6792179025</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>